<commit_message>
correções dos factor que eram pra ser numéricos e correlacao no script.r
</commit_message>
<xml_diff>
--- a/datasets/access_to_improved_sanitation.xlsx
+++ b/datasets/access_to_improved_sanitation.xlsx
@@ -1943,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:AH246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AI1" sqref="AI1:AI1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>